<commit_message>
Adds paper. Updates proposal.
</commit_message>
<xml_diff>
--- a/Proposal/Milestones.xlsx
+++ b/Proposal/Milestones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanwinter/Local/Thesis/Proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E16095F-6994-5447-BF5E-93BC4CDE5EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82EE0B9-F475-2F4B-8875-99A5990DC7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4340" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A5961234-51F8-2E43-9D90-E0419C5AE6D8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A5961234-51F8-2E43-9D90-E0419C5AE6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="GANTT" sheetId="2" r:id="rId1"/>
@@ -148,13 +148,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -270,34 +270,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,6 +484,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-12F3-5543-90C6-16C90966CBB6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -557,10 +562,6 @@
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
@@ -674,10 +675,6 @@
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
@@ -737,10 +734,6 @@
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
@@ -797,10 +790,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -868,37 +857,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>116</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,551 +1087,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1687,16 +1131,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD3A983A-34CC-B642-ABB1-45B29C606271}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD3A983A-34CC-B642-ABB1-45B29C606271}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:F12" xr:uid="{182E5482-ABAB-A24C-B417-48C62BEF9293}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A325299B-D988-6F4B-81B5-51198A333671}" name="Task"/>
     <tableColumn id="4" xr3:uid="{5248C2D5-1D57-1842-A29F-BB88789AED41}" name="Category"/>
     <tableColumn id="2" xr3:uid="{0D65C1B4-0321-5A43-9A46-0284C9378EAC}" name="Days From Now"/>
-    <tableColumn id="3" xr3:uid="{4A8ABD7F-4B33-6848-9886-AD97EED227AA}" name="Days To Complete Milestone" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{4A8ABD7F-4B33-6848-9886-AD97EED227AA}" name="Days To Complete Milestone" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1F3DC285-7831-FF4E-B7FF-CC806C006119}" name="Start Date" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{1F3DC285-7831-FF4E-B7FF-CC806C006119}" name="Start Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2021,10,28)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{DAA3444F-FDED-E845-AF97-E1FF41D18A60}" name="End Date"/>
@@ -2005,7 +1449,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2049,11 +1493,11 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44466</v>
+        <v>44467</v>
       </c>
       <c r="F2" s="1">
         <f>DATE(2021,10,1)</f>
@@ -2069,19 +1513,18 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">Table1[[#This Row],[Start Date]]-TODAY()</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1">
         <f>DATE(2021,10,8)</f>
         <v>44477</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3" si="0">DATE(2021,10,15)</f>
-        <v>44484</v>
+        <v>44479</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2093,11 +1536,11 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">Table1[[#This Row],[Start Date]]-TODAY()</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1">
         <f>DATE(2021,10,21)</f>
@@ -2117,19 +1560,17 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">Table1[[#This Row],[Start Date]]-TODAY()</f>
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1">
-        <f>DATE(2021,10,15)</f>
-        <v>44484</v>
+        <v>44468</v>
       </c>
       <c r="F5" s="1">
-        <f>DATE(2021,11,5)</f>
-        <v>44505</v>
+        <v>44508</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2141,19 +1582,17 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">Table1[[#This Row],[Start Date]]-TODAY()</f>
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1">
-        <f>DATE(2021,10,31)</f>
-        <v>44500</v>
+        <v>44468</v>
       </c>
       <c r="F6" s="1">
-        <f>DATE(2021,11,5)</f>
-        <v>44505</v>
+        <v>44508</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2165,11 +1604,11 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">Table1[[#This Row],[Start Date]]-TODAY()</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1">
         <f>DATE(2021,11,5)</f>
@@ -2189,11 +1628,11 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">IF(Table1[[#This Row],[Start Date]]-TODAY()&gt;0,Table1[[#This Row],[Start Date]]-TODAY(),0)</f>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1">
         <f>DATE(2021,11,19)</f>
@@ -2213,11 +1652,11 @@
       </c>
       <c r="C9" s="2">
         <f ca="1">IF(Table1[[#This Row],[Start Date]]-TODAY()&gt;0,Table1[[#This Row],[Start Date]]-TODAY(),0)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1">
         <f>DATE(2021,11,23)</f>
@@ -2237,11 +1676,11 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">IF(Table1[[#This Row],[Start Date]]-TODAY()&gt;0,Table1[[#This Row],[Start Date]]-TODAY(),0)</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="1">
         <f>DATE(2021,11,26)</f>
@@ -2261,11 +1700,11 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">IF(Table1[[#This Row],[Start Date]]-TODAY()&gt;0,Table1[[#This Row],[Start Date]]-TODAY(),0)</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1">
         <f>DATE(2021,11,29)</f>
@@ -2285,11 +1724,11 @@
       </c>
       <c r="C12" s="2">
         <f ca="1">IF(Table1[[#This Row],[Start Date]]-TODAY()&gt;0,Table1[[#This Row],[Start Date]]-TODAY(),0)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="2">
         <f ca="1">Table1[[#This Row],[End Date]]-Table1[[#This Row],[Start Date]]+Table1[[#This Row],[Days From Now]]</f>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="1">
         <f>DATE(2021,12,28)</f>

</xml_diff>